<commit_message>
Updated code for Account check and Rcore API
Successfully executed account check flow with screenshots features
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="77">
   <si>
     <t>RestAddBook</t>
   </si>
@@ -235,6 +235,18 @@
   </si>
   <si>
     <t>"4g6"</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Account.bank2</t>
+  </si>
+  <si>
+    <t>bank2</t>
   </si>
 </sst>
 </file>
@@ -603,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +638,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -684,8 +696,14 @@
       <c r="S1" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -743,8 +761,14 @@
       <c r="S2" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -803,7 +827,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -862,7 +886,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -921,7 +945,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -980,7 +1004,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1039,7 +1063,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1098,7 +1122,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1157,7 +1181,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1216,7 +1240,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1275,7 +1299,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1334,7 +1358,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1393,7 +1417,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1452,7 +1476,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1511,7 +1535,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
RestAssuredMaven with Allure Reporting
RestAssuredMaven with Allure Reporting and also used @FindBy instead of By in Account check portal page.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -11,12 +11,12 @@
     <sheet name="RestAssured" sheetId="2" r:id="rId2"/>
     <sheet name="example" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="81">
   <si>
     <t>RestAddBook</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>bank2</t>
+  </si>
+  <si>
+    <t>AccountChek.bank18</t>
+  </si>
+  <si>
+    <t>bank18</t>
+  </si>
+  <si>
+    <t>Username2</t>
+  </si>
+  <si>
+    <t>Password2</t>
   </si>
 </sst>
 </file>
@@ -615,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="V2" sqref="V2:W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,10 +647,12 @@
     <col min="13" max="13" width="22" style="1" customWidth="1"/>
     <col min="14" max="16" width="22.5703125" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.28515625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -702,8 +716,14 @@
       <c r="U1" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -767,8 +787,14 @@
       <c r="U2" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -826,8 +852,20 @@
       <c r="S3" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -885,8 +923,20 @@
       <c r="S4" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -944,8 +994,20 @@
       <c r="S5" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1003,8 +1065,20 @@
       <c r="S6" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1063,7 +1137,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1122,7 +1196,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1181,7 +1255,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1240,7 +1314,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1299,7 +1373,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1358,7 +1432,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1417,7 +1491,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1476,7 +1550,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1535,7 +1609,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
With Read Config and Plaid Test cases
With Read Config and Plaid Test cases.
Added RC properties and also completed refactoring for account check.
Also added Drivers, Utilities and Configuration folders
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AccountCheck" sheetId="1" r:id="rId1"/>
-    <sheet name="RestAssured" sheetId="2" r:id="rId2"/>
-    <sheet name="example" sheetId="3" r:id="rId3"/>
+    <sheet name="Plaid" sheetId="4" r:id="rId2"/>
+    <sheet name="RestAssured" sheetId="2" r:id="rId3"/>
+    <sheet name="example" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="129">
   <si>
     <t>RestAddBook</t>
   </si>
@@ -259,6 +260,150 @@
   </si>
   <si>
     <t>Password2</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Valild Plaid Flow with all parameters</t>
+  </si>
+  <si>
+    <t>"PLAID"</t>
+  </si>
+  <si>
+    <t>"https://acme-lending.com/redirectHandler"</t>
+  </si>
+  <si>
+    <t>"https://webhook.site/0221d600-6d3c-49f3-828a-35b635624c1d"</t>
+  </si>
+  <si>
+    <t>"Test"</t>
+  </si>
+  <si>
+    <t>"Data"</t>
+  </si>
+  <si>
+    <t>"test@test.test"</t>
+  </si>
+  <si>
+    <t>"test"</t>
+  </si>
+  <si>
+    <t>"tester"</t>
+  </si>
+  <si>
+    <t>"123, address"</t>
+  </si>
+  <si>
+    <t>"84101"</t>
+  </si>
+  <si>
+    <t>Valild Plaid Flow with only mandatory parameters</t>
+  </si>
+  <si>
+    <t>Null Zip Code</t>
+  </si>
+  <si>
+    <t>Null Address line 1</t>
+  </si>
+  <si>
+    <t>Null Last Name</t>
+  </si>
+  <si>
+    <t>Null SSN</t>
+  </si>
+  <si>
+    <t>Null email address</t>
+  </si>
+  <si>
+    <t>Null First Name</t>
+  </si>
+  <si>
+    <t>SSN less than 9 digits</t>
+  </si>
+  <si>
+    <t>SSN greater than 9 digits</t>
+  </si>
+  <si>
+    <t>Invalid email address1</t>
+  </si>
+  <si>
+    <t>Invalid email address2</t>
+  </si>
+  <si>
+    <t>"test@test"</t>
+  </si>
+  <si>
+    <t>Invalid email address3</t>
+  </si>
+  <si>
+    <t>"test.test"</t>
+  </si>
+  <si>
+    <t>Invalid email address4</t>
+  </si>
+  <si>
+    <t>"1234"</t>
+  </si>
+  <si>
+    <t>Invalid email address5</t>
+  </si>
+  <si>
+    <t>"test()*g@hyug.gy"</t>
+  </si>
+  <si>
+    <t>Invalid Zip Code</t>
+  </si>
+  <si>
+    <t>Invalid customer_id</t>
+  </si>
+  <si>
+    <t>Invalid account_id</t>
+  </si>
+  <si>
+    <t>Null customer_id</t>
+  </si>
+  <si>
+    <t>Null account_id</t>
+  </si>
+  <si>
+    <t>Invalid verification_type</t>
+  </si>
+  <si>
+    <t>Null verification_type</t>
+  </si>
+  <si>
+    <t>Null first name, last name, ssn</t>
+  </si>
+  <si>
+    <t>zip code less than 5 digits, ssn less than 9, null fist and last name, invalid email</t>
+  </si>
+  <si>
+    <t>"test.com"</t>
+  </si>
+  <si>
+    <t>"8410"</t>
+  </si>
+  <si>
+    <t>Null cust_id and ac-id</t>
+  </si>
+  <si>
+    <t>Invalid cust_id, ac_id</t>
+  </si>
+  <si>
+    <t>"839e7e29-3d7f-4aa5-9ae7-94d6d4f1ec7"</t>
+  </si>
+  <si>
+    <t>"PLAI"</t>
+  </si>
+  <si>
+    <t>user_good</t>
+  </si>
+  <si>
+    <t>pass_good</t>
   </si>
 </sst>
 </file>
@@ -629,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:W6"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,6 +2419,1451 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1"/>
+    <col min="7" max="7" width="57.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="1">
+        <v>200</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="1">
+        <v>200</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="1">
+        <v>200</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="1">
+        <v>123456790</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P5" s="1">
+        <v>200</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P6" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P7" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P8" s="1">
+        <v>200</v>
+      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K10" s="1">
+        <v>123456</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P10" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K11" s="1">
+        <v>12345678901</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P11" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K12" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P12" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K13" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P13" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P14" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K15" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P15" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K18" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18" s="1">
+        <v>500</v>
+      </c>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P19" s="1">
+        <v>500</v>
+      </c>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K20" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P20" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K21" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P21" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K22" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P22" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K23" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P23" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P24" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K25" s="1">
+        <v>12345678</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P25" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K26" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" s="1">
+        <v>400</v>
+      </c>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P27" s="1">
+        <v>500</v>
+      </c>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2327,7 +3917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>